<commit_message>
Pre screwing around with the functions managing certificate generation.  in a testing state
</commit_message>
<xml_diff>
--- a/SNA Certificate Checklist.xlsx
+++ b/SNA Certificate Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamunson\Documents\PythonProjects\CSRCreator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C57D5A1-23A4-496E-AE95-026776B37424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E73A5D-255E-405B-AFB4-D26A8140C86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="495" windowWidth="16035" windowHeight="13545" xr2:uid="{4382B469-41DA-4883-923D-A2AB46E6C898}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Hostname</t>
   </si>
@@ -100,6 +100,30 @@
   </si>
   <si>
     <t>smc-02.domain.com</t>
+  </si>
+  <si>
+    <t>IP Address</t>
+  </si>
+  <si>
+    <t>10.10.10.112</t>
+  </si>
+  <si>
+    <t>10.10.10.161</t>
+  </si>
+  <si>
+    <t>10.10.10.40</t>
+  </si>
+  <si>
+    <t>10.10.10.85</t>
+  </si>
+  <si>
+    <t>10.10.10.27</t>
+  </si>
+  <si>
+    <t>10.10.10.187</t>
+  </si>
+  <si>
+    <t>10.10.10.230</t>
   </si>
 </sst>
 </file>
@@ -516,180 +540,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DA0C31-6692-4377-BE41-3CB05727CEC1}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" customWidth="1"/>
-    <col min="5" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" customWidth="1"/>
+    <col min="6" max="11" width="4.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="95.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="95.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="4"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="3"/>
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="3"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="3"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="3"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="N9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed SAN Fields in CSR
</commit_message>
<xml_diff>
--- a/SNA Certificate Checklist.xlsx
+++ b/SNA Certificate Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamunson\Documents\PythonProjects\CSRCreator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E73A5D-255E-405B-AFB4-D26A8140C86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D06B58-BD36-4DD3-9A2A-8B2160962D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="495" windowWidth="16035" windowHeight="13545" xr2:uid="{4382B469-41DA-4883-923D-A2AB46E6C898}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Hostname</t>
   </si>
@@ -112,12 +112,6 @@
   </si>
   <si>
     <t>10.10.10.40</t>
-  </si>
-  <si>
-    <t>10.10.10.85</t>
-  </si>
-  <si>
-    <t>10.10.10.27</t>
   </si>
   <si>
     <t>10.10.10.187</t>
@@ -543,7 +537,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,9 +645,7 @@
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
@@ -671,9 +663,7 @@
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
@@ -692,7 +682,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>10</v>
@@ -732,7 +722,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>

</xml_diff>